<commit_message>
fetched latest from origin
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataExcel.xlsx
+++ b/src/test/resources/TestDataExcel.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>URL</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>₹53,990</t>
+  </si>
+  <si>
+    <t>₹38,990</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A6AA5B1-BD7F-47D9-8A01-64EDE7847C06}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -478,6 +481,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>